<commit_message>
Added NetworkX as a backend for plotting the graph
</commit_message>
<xml_diff>
--- a/T32 preceptor profiles_collaborators.xlsx
+++ b/T32 preceptor profiles_collaborators.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adel/code/collaborationGraphVisualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$1:$C$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$D$1:$D$33</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="275">
   <si>
     <t>Faculty</t>
   </si>
@@ -580,10 +580,283 @@
     <t>Robinson, Sinha, Vasudevan, Zhu</t>
   </si>
   <si>
-    <t>Zhu, Ruoqing</t>
-  </si>
-  <si>
-    <t>Qu, Peiyong  (Annie)</t>
+    <t>Degnan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Patrick</t>
+  </si>
+  <si>
+    <t>Hudson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Matthew</t>
+  </si>
+  <si>
+    <t>Cann</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac K O</t>
+  </si>
+  <si>
+    <t>Mendenhall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ruby</t>
+  </si>
+  <si>
+    <t>Uddin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monica</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gene</t>
+  </si>
+  <si>
+    <t>Whitaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rachel</t>
+  </si>
+  <si>
+    <t>Wildman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Derek</t>
+  </si>
+  <si>
+    <t>Stubbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lisa</t>
+  </si>
+  <si>
+    <t>Metcalf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bill</t>
+  </si>
+  <si>
+    <t>Song</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jun</t>
+  </si>
+  <si>
+    <t>Bagchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Milan</t>
+  </si>
+  <si>
+    <t>Brunner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robert</t>
+  </si>
+  <si>
+    <t>Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Deming</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Minh</t>
+  </si>
+  <si>
+    <t>Hart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> John</t>
+  </si>
+  <si>
+    <t>Iyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ravishankar K</t>
+  </si>
+  <si>
+    <t>Peng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jian</t>
+  </si>
+  <si>
+    <t>Sinha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Saurabh</t>
+  </si>
+  <si>
+    <t>Vasudevan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shobha</t>
+  </si>
+  <si>
+    <t>Han</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jiawei</t>
+  </si>
+  <si>
+    <t>Roth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dan</t>
+  </si>
+  <si>
+    <t>Maslov</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sergei</t>
+  </si>
+  <si>
+    <t>Nagi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rakesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sandra Luisa</t>
+  </si>
+  <si>
+    <t>Zhao</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sihai Dave</t>
+  </si>
+  <si>
+    <t>Villamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maria Bonita</t>
+  </si>
+  <si>
+    <t>Caetano-Anolles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gustavo</t>
+  </si>
+  <si>
+    <t>Qu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peiyong  (Annie)</t>
+  </si>
+  <si>
+    <t>Zhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ruoqing</t>
+  </si>
+  <si>
+    <t>Rosu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luisa-Maria</t>
+  </si>
+  <si>
+    <t>Stodden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Victoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whitaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wildman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Metcalf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sinha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mendenhall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maslov</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uddin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rodriguez-Zas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rodriguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cann</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Degnan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hudson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Qu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vasudevan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zhu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zhao</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bagchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Han</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Song</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Campbell</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stubbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Villamil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Caetano</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zhu</t>
   </si>
 </sst>
 </file>
@@ -2313,308 +2586,619 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="60.1640625" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="41"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="41"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="41"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="41"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>188</v>
+      </c>
+      <c r="B4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5" s="41"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="C6" s="41"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+        <v>192</v>
+      </c>
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" t="s">
+        <v>256</v>
+      </c>
+      <c r="G6" t="s">
+        <v>251</v>
+      </c>
+      <c r="H6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="41"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+      <c r="B7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="E7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="41"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G8" t="s">
+        <v>252</v>
+      </c>
+      <c r="H8" t="s">
+        <v>260</v>
+      </c>
+      <c r="I8" t="s">
+        <v>256</v>
+      </c>
+      <c r="J8" t="s">
+        <v>261</v>
+      </c>
+      <c r="K8" t="s">
+        <v>254</v>
+      </c>
+      <c r="L8" t="s">
+        <v>232</v>
+      </c>
+      <c r="M8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="41"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="41"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+      <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="41"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+        <v>202</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="41"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+      <c r="B12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="41"/>
+        <v>206</v>
+      </c>
+      <c r="B13" t="s">
+        <v>207</v>
+      </c>
       <c r="C13" s="41"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D13" s="41"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C14" s="41"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="41"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="41"/>
+        <v>213</v>
+      </c>
+      <c r="B17" t="s">
+        <v>214</v>
+      </c>
       <c r="C17" s="41"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="41"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" t="s">
+        <v>249</v>
+      </c>
+      <c r="F18" t="s">
+        <v>247</v>
+      </c>
+      <c r="G18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="41"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+      <c r="B19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="41"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+        <v>219</v>
+      </c>
+      <c r="B20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="E20" t="s">
+        <v>267</v>
+      </c>
+      <c r="F20" t="s">
+        <v>268</v>
+      </c>
+      <c r="G20" t="s">
+        <v>259</v>
+      </c>
+      <c r="H20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>172</v>
-      </c>
-      <c r="C21" s="41"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+      <c r="B21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="E21" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" t="s">
+        <v>266</v>
+      </c>
+      <c r="G21" t="s">
+        <v>247</v>
+      </c>
+      <c r="H21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C22" s="41"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+        <v>223</v>
+      </c>
+      <c r="B22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="E22" t="s">
+        <v>266</v>
+      </c>
+      <c r="F22" t="s">
+        <v>251</v>
+      </c>
+      <c r="G22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="41"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+        <v>225</v>
+      </c>
+      <c r="B23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="41"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+      <c r="B24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="41"/>
+        <v>229</v>
+      </c>
+      <c r="B25" t="s">
+        <v>230</v>
+      </c>
       <c r="C25" s="41"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D25" s="41"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+        <v>171</v>
+      </c>
+      <c r="B26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="E26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F26" t="s">
+        <v>271</v>
+      </c>
+      <c r="G26" t="s">
+        <v>270</v>
+      </c>
+      <c r="H26" t="s">
+        <v>251</v>
+      </c>
+      <c r="I26" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" t="s">
+        <v>272</v>
+      </c>
+      <c r="K26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="C27" s="41"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+        <v>232</v>
+      </c>
+      <c r="B27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" t="s">
+        <v>261</v>
+      </c>
+      <c r="F27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="41"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D28" s="41"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C29" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="41"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="C30" s="41"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+      <c r="B30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="41"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+        <v>240</v>
+      </c>
+      <c r="B31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="E31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="B32" s="41"/>
+        <v>242</v>
+      </c>
+      <c r="B32" t="s">
+        <v>243</v>
+      </c>
       <c r="C32" s="41"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D32" s="41"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="41"/>
+        <v>244</v>
+      </c>
+      <c r="B33" t="s">
+        <v>245</v>
+      </c>
       <c r="C33" s="41"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="41"/>
+      <c r="D33" s="41"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B34" s="41"/>
       <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>